<commit_message>
does this do anything?
</commit_message>
<xml_diff>
--- a/_archive/PATH 2019 Q3 LRF Meeting _CE (1).xlsx
+++ b/_archive/PATH 2019 Q3 LRF Meeting _CE (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chriseshleman/Dropbox/Work and research/Port Authority/pathforecast/_archive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B6C5BA2-DE36-324D-863D-68319D1632DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E680B4-68DD-784D-98DE-126982CF7F70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="5820" windowWidth="23880" windowHeight="15180" activeTab="4" xr2:uid="{4B786C43-CFFF-4E2C-8222-145C0B96F105}"/>
+    <workbookView xWindow="1960" yWindow="1660" windowWidth="23880" windowHeight="15180" activeTab="4" xr2:uid="{4B786C43-CFFF-4E2C-8222-145C0B96F105}"/>
   </bookViews>
   <sheets>
     <sheet name="1 and 2 - PAX Comparison" sheetId="1" r:id="rId1"/>
@@ -935,7 +935,7 @@
     <numFmt numFmtId="175" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
-  <fonts count="50" x14ac:knownFonts="1">
+  <fonts count="50">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2201,7 +2201,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="329">
+  <cellXfs count="331">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2555,6 +2555,8 @@
     <xf numFmtId="164" fontId="49" fillId="29" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="49" fillId="29" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="8" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="8" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7578,7 +7580,7 @@
       <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40" style="153" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" style="153" bestFit="1" customWidth="1"/>
@@ -7589,7 +7591,7 @@
     <col min="18" max="22" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="19">
       <c r="A1" s="196" t="s">
         <v>86</v>
       </c>
@@ -7615,7 +7617,7 @@
       <c r="U1" s="292"/>
       <c r="V1" s="292"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2" s="155"/>
@@ -7638,7 +7640,7 @@
       <c r="U2" s="155"/>
       <c r="V2" s="155"/>
     </row>
-    <row r="3" spans="1:22" s="153" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" s="153" customFormat="1">
       <c r="A3" s="159" t="s">
         <v>90</v>
       </c>
@@ -7724,7 +7726,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="176" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" s="176" customFormat="1">
       <c r="A4" s="175" t="s">
         <v>35</v>
       </c>
@@ -7813,7 +7815,7 @@
         <v>105751921.41749577</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="157" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" s="157" customFormat="1">
       <c r="A5" s="166" t="s">
         <v>34</v>
       </c>
@@ -7834,7 +7836,7 @@
         <v>-2698300</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" s="156" customFormat="1">
       <c r="A6" s="154" t="s">
         <v>36</v>
       </c>
@@ -7905,7 +7907,7 @@
         <v>105751921.41749577</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="158" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" s="158" customFormat="1">
       <c r="B7" s="166"/>
       <c r="C7" s="166"/>
       <c r="D7" s="165"/>
@@ -7982,7 +7984,7 @@
         <v>1.3047065340338726E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="162" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" s="162" customFormat="1">
       <c r="A8" s="160" t="s">
         <v>104</v>
       </c>
@@ -8071,7 +8073,7 @@
         <v>-2879540.7910995781</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="164" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" s="164" customFormat="1">
       <c r="A9" s="154" t="s">
         <v>31</v>
       </c>
@@ -8142,7 +8144,7 @@
         <v>102872380.62639619</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="158" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" s="158" customFormat="1">
       <c r="B10" s="167"/>
       <c r="C10" s="167"/>
       <c r="D10" s="165">
@@ -8222,7 +8224,7 @@
         <v>1.0378819600476374E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="162" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" s="162" customFormat="1">
       <c r="A11" s="160" t="s">
         <v>105</v>
       </c>
@@ -8311,7 +8313,7 @@
         <v>-1106956.3993516117</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="164" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" s="164" customFormat="1">
       <c r="A12" s="154" t="s">
         <v>32</v>
       </c>
@@ -8382,7 +8384,7 @@
         <v>101765424.22704458</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="158" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" s="158" customFormat="1">
       <c r="B13" s="167"/>
       <c r="C13" s="167"/>
       <c r="D13" s="165">
@@ -8462,7 +8464,7 @@
         <v>1.0292896583099953E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="162" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" s="162" customFormat="1">
       <c r="A14" s="160" t="s">
         <v>106</v>
       </c>
@@ -8551,7 +8553,7 @@
         <v>-1091596.9964554012</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="164" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" s="164" customFormat="1">
       <c r="A15" s="154" t="s">
         <v>37</v>
       </c>
@@ -8622,7 +8624,7 @@
         <v>100673827.23058918</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="158" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" s="158" customFormat="1">
       <c r="B16" s="167"/>
       <c r="C16" s="167"/>
       <c r="D16" s="165">
@@ -8702,7 +8704,7 @@
         <v>9.8391193882683137E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="166" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" s="166" customFormat="1">
       <c r="A17" s="166" t="s">
         <v>39</v>
       </c>
@@ -8723,7 +8725,7 @@
         <v>-2700000</v>
       </c>
     </row>
-    <row r="18" spans="1:22" s="174" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" s="174" customFormat="1">
       <c r="A18" s="174" t="s">
         <v>38</v>
       </c>
@@ -8812,8 +8814,8 @@
         <v>100673827.23058918</v>
       </c>
     </row>
-    <row r="19" spans="1:22" s="166" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:22" s="168" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" s="166" customFormat="1"/>
+    <row r="20" spans="1:22" s="168" customFormat="1">
       <c r="A20" s="172" t="s">
         <v>33</v>
       </c>
@@ -8902,7 +8904,7 @@
         <v>-5078094.1869065911</v>
       </c>
     </row>
-    <row r="21" spans="1:22" s="170" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" s="170" customFormat="1">
       <c r="A21" s="168" t="s">
         <v>107</v>
       </c>
@@ -8991,107 +8993,107 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" s="156" customFormat="1">
       <c r="A22" s="154"/>
       <c r="B22" s="166"/>
       <c r="C22" s="166"/>
     </row>
-    <row r="23" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" s="156" customFormat="1">
       <c r="A23" s="154"/>
       <c r="B23" s="166"/>
       <c r="C23" s="166"/>
     </row>
-    <row r="24" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" s="156" customFormat="1">
       <c r="A24" s="154"/>
       <c r="B24" s="166"/>
       <c r="C24" s="166"/>
     </row>
-    <row r="25" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" s="156" customFormat="1">
       <c r="A25" s="154"/>
       <c r="B25" s="166"/>
       <c r="C25" s="166"/>
     </row>
-    <row r="26" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" s="156" customFormat="1">
       <c r="A26" s="154"/>
       <c r="B26" s="166"/>
       <c r="C26" s="166"/>
     </row>
-    <row r="27" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" s="156" customFormat="1">
       <c r="A27" s="154"/>
       <c r="B27" s="166"/>
       <c r="C27" s="166"/>
     </row>
-    <row r="28" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" s="156" customFormat="1">
       <c r="A28" s="154"/>
       <c r="B28" s="166"/>
       <c r="C28" s="166"/>
     </row>
-    <row r="29" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" s="156" customFormat="1">
       <c r="A29" s="154"/>
       <c r="B29" s="166"/>
       <c r="C29" s="166"/>
     </row>
-    <row r="30" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" s="156" customFormat="1">
       <c r="A30" s="154"/>
       <c r="B30" s="166"/>
       <c r="C30" s="166"/>
     </row>
-    <row r="31" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" s="156" customFormat="1">
       <c r="A31" s="154"/>
       <c r="B31" s="154"/>
       <c r="C31" s="154"/>
     </row>
-    <row r="32" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" s="156" customFormat="1">
       <c r="A32" s="154"/>
       <c r="B32" s="154"/>
       <c r="C32" s="154"/>
     </row>
-    <row r="33" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" s="156" customFormat="1">
       <c r="A33" s="154"/>
       <c r="B33" s="154"/>
       <c r="C33" s="154"/>
     </row>
-    <row r="34" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" s="156" customFormat="1">
       <c r="A34" s="154"/>
       <c r="B34" s="154"/>
       <c r="C34" s="154"/>
     </row>
-    <row r="35" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" s="156" customFormat="1">
       <c r="A35" s="154"/>
       <c r="B35" s="154"/>
       <c r="C35" s="154"/>
     </row>
-    <row r="36" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" s="156" customFormat="1">
       <c r="A36" s="154"/>
       <c r="B36" s="154"/>
       <c r="C36" s="154"/>
     </row>
-    <row r="37" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" s="156" customFormat="1">
       <c r="A37" s="154"/>
       <c r="B37" s="154"/>
       <c r="C37" s="154"/>
     </row>
-    <row r="38" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" s="156" customFormat="1">
       <c r="A38" s="154"/>
       <c r="B38" s="154"/>
       <c r="C38" s="154"/>
     </row>
-    <row r="39" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" s="156" customFormat="1">
       <c r="A39" s="154"/>
       <c r="B39" s="154"/>
       <c r="C39" s="154"/>
     </row>
-    <row r="40" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" s="156" customFormat="1">
       <c r="A40" s="154"/>
       <c r="B40" s="154"/>
       <c r="C40" s="154"/>
     </row>
-    <row r="41" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" s="156" customFormat="1">
       <c r="A41" s="154"/>
       <c r="B41" s="154"/>
       <c r="C41" s="154"/>
     </row>
-    <row r="42" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" s="156" customFormat="1">
       <c r="A42" s="270" t="s">
         <v>88</v>
       </c>
@@ -9159,7 +9161,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="43" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" s="156" customFormat="1">
       <c r="A43" s="271" t="s">
         <v>91</v>
       </c>
@@ -9229,7 +9231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" s="156" customFormat="1">
       <c r="A44" s="271"/>
       <c r="B44" s="271"/>
       <c r="D44" s="273"/>
@@ -9306,7 +9308,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" s="156" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" s="156" customFormat="1">
       <c r="A45" s="271" t="s">
         <v>92</v>
       </c>
@@ -9376,7 +9378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22">
       <c r="A46" s="271"/>
       <c r="B46" s="271"/>
       <c r="D46" s="273"/>
@@ -9453,7 +9455,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22">
       <c r="A47" s="275" t="s">
         <v>45</v>
       </c>
@@ -9535,7 +9537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22">
       <c r="A48" s="277"/>
       <c r="B48" s="277"/>
       <c r="D48" s="278"/>
@@ -9612,7 +9614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:31">
       <c r="A49" s="271"/>
       <c r="B49" s="271"/>
       <c r="D49" s="273"/>
@@ -9635,7 +9637,7 @@
       <c r="U49" s="273"/>
       <c r="V49" s="273"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:31">
       <c r="A50" s="271" t="s">
         <v>93</v>
       </c>
@@ -9705,7 +9707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:31">
       <c r="A51" s="271"/>
       <c r="B51" s="271"/>
       <c r="D51" s="273"/>
@@ -9782,7 +9784,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:31">
       <c r="A52" s="271" t="s">
         <v>94</v>
       </c>
@@ -9852,7 +9854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:31">
       <c r="A53" s="271"/>
       <c r="B53" s="271"/>
       <c r="D53" s="273"/>
@@ -9929,7 +9931,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:31">
       <c r="A54" s="275" t="s">
         <v>45</v>
       </c>
@@ -10010,7 +10012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:31">
       <c r="E55" s="279">
         <f t="shared" ref="E55:V55" si="124">E53-E51</f>
         <v>-8.399154421177002E-4</v>
@@ -10084,7 +10086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:31">
       <c r="A57" s="159"/>
       <c r="B57" s="159"/>
       <c r="C57" s="159" t="s">
@@ -10203,7 +10205,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:31">
       <c r="A58" s="153" t="s">
         <v>96</v>
       </c>
@@ -10315,7 +10317,7 @@
         <v>99692936.525943369</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:31">
       <c r="D59" s="269"/>
       <c r="E59" s="165">
         <f>E58/D58-1</f>
@@ -10440,7 +10442,7 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.6640625" style="153" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
@@ -10453,12 +10455,12 @@
     <col min="13" max="22" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29 16378:16378" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29 16378:16378" ht="19">
       <c r="A1" s="196" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:29 16378:16378" s="180" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29 16378:16378" s="180" customFormat="1">
       <c r="A3" s="153" t="s">
         <v>40</v>
       </c>
@@ -10533,7 +10535,7 @@
       <c r="AB3" s="177"/>
       <c r="AC3" s="177"/>
     </row>
-    <row r="4" spans="1:29 16378:16378" s="177" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29 16378:16378" s="177" customFormat="1">
       <c r="A4" s="181" t="s">
         <v>3</v>
       </c>
@@ -10601,7 +10603,7 @@
         <v>416.79146403167869</v>
       </c>
     </row>
-    <row r="5" spans="1:29 16378:16378" s="185" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29 16378:16378" s="185" customFormat="1">
       <c r="A5" s="183" t="s">
         <v>41</v>
       </c>
@@ -10687,7 +10689,7 @@
         <v>2.1723594982906436E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:29 16378:16378" s="177" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29 16378:16378" s="177" customFormat="1">
       <c r="A6" s="181"/>
       <c r="B6" s="186"/>
       <c r="C6" s="186"/>
@@ -10711,7 +10713,7 @@
       <c r="U6" s="181"/>
       <c r="V6" s="181"/>
     </row>
-    <row r="7" spans="1:29 16378:16378" s="153" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29 16378:16378" s="153" customFormat="1">
       <c r="A7" s="183" t="s">
         <v>42</v>
       </c>
@@ -10799,7 +10801,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="8" spans="1:29 16378:16378" s="185" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29 16378:16378" s="185" customFormat="1">
       <c r="A8" s="187"/>
       <c r="B8" s="188"/>
       <c r="C8" s="188"/>
@@ -10881,7 +10883,7 @@
       </c>
       <c r="XEX8" s="189"/>
     </row>
-    <row r="10" spans="1:29 16378:16378" s="153" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29 16378:16378" s="153" customFormat="1">
       <c r="A10" s="181" t="s">
         <v>43</v>
       </c>
@@ -10969,7 +10971,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="11" spans="1:29 16378:16378" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29 16378:16378">
       <c r="B11" s="190"/>
       <c r="C11" s="190"/>
       <c r="D11" s="190"/>
@@ -10992,7 +10994,7 @@
       <c r="U11" s="190"/>
       <c r="V11" s="190"/>
     </row>
-    <row r="12" spans="1:29 16378:16378" s="192" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29 16378:16378" s="192" customFormat="1">
       <c r="A12" s="183" t="s">
         <v>44</v>
       </c>
@@ -11078,7 +11080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:29 16378:16378" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29 16378:16378" ht="16" thickBot="1">
       <c r="B13" s="190"/>
       <c r="C13" s="193"/>
       <c r="D13" s="193"/>
@@ -11100,7 +11102,7 @@
       <c r="U13" s="190"/>
       <c r="V13" s="190"/>
     </row>
-    <row r="14" spans="1:29 16378:16378" s="153" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29 16378:16378" s="153" customFormat="1" ht="16" thickBot="1">
       <c r="A14" s="261" t="s">
         <v>102</v>
       </c>
@@ -11185,8 +11187,8 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="15" spans="1:29 16378:16378" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:29 16378:16378" s="153" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29 16378:16378" ht="16" thickBot="1"/>
+    <row r="16" spans="1:29 16378:16378" s="153" customFormat="1" ht="16" thickBot="1">
       <c r="A16" s="263" t="s">
         <v>101</v>
       </c>
@@ -11272,7 +11274,7 @@
         <v>3.5486222936743741</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="259" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" s="259" customFormat="1">
       <c r="A17" s="258"/>
       <c r="C17" s="260"/>
       <c r="D17" s="165"/>
@@ -11295,7 +11297,7 @@
       <c r="U17" s="165"/>
       <c r="V17" s="165"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22">
       <c r="A18" s="195" t="s">
         <v>103</v>
       </c>
@@ -11396,7 +11398,7 @@
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="32.6640625" style="199" customWidth="1"/>
     <col min="2" max="2" width="1.5" style="199" customWidth="1"/>
@@ -11413,42 +11415,42 @@
     <col min="26" max="16384" width="9.33203125" style="199"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="18">
       <c r="A1" s="265" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:23" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" hidden="1" outlineLevel="1">
       <c r="A2" s="198" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:23" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" hidden="1" outlineLevel="1">
       <c r="A3" s="198" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:23" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" hidden="1" outlineLevel="1">
       <c r="A4" s="200">
         <v>43697</v>
       </c>
     </row>
-    <row r="5" spans="1:23" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" hidden="1" outlineLevel="1">
       <c r="A5" s="201" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:23" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:23" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="299" t="s">
+    <row r="6" spans="1:23" hidden="1" outlineLevel="1"/>
+    <row r="7" spans="1:23" hidden="1" outlineLevel="1">
+      <c r="C7" s="301" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="299"/>
-      <c r="E7" s="299"/>
-      <c r="F7" s="299"/>
-      <c r="G7" s="299"/>
-    </row>
-    <row r="8" spans="1:23" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="301"/>
+      <c r="E7" s="301"/>
+      <c r="F7" s="301"/>
+      <c r="G7" s="301"/>
+    </row>
+    <row r="8" spans="1:23" hidden="1" outlineLevel="1">
       <c r="C8" s="203">
         <v>2019</v>
       </c>
@@ -11487,7 +11489,7 @@
       <c r="S8" s="246"/>
       <c r="T8" s="246"/>
     </row>
-    <row r="9" spans="1:23" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" hidden="1" outlineLevel="1">
       <c r="A9" s="204"/>
       <c r="C9" s="205" t="s">
         <v>56</v>
@@ -11529,7 +11531,7 @@
       <c r="V9" s="207"/>
       <c r="W9" s="208"/>
     </row>
-    <row r="10" spans="1:23" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" hidden="1" outlineLevel="1">
       <c r="A10" s="201" t="s">
         <v>59</v>
       </c>
@@ -11573,7 +11575,7 @@
       <c r="V10" s="207"/>
       <c r="W10" s="208"/>
     </row>
-    <row r="11" spans="1:23" ht="17" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="17" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A11" s="201" t="s">
         <v>50</v>
       </c>
@@ -11613,7 +11615,7 @@
       <c r="V11" s="207"/>
       <c r="W11" s="208"/>
     </row>
-    <row r="12" spans="1:23" ht="17" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="17" hidden="1" outlineLevel="1" thickTop="1">
       <c r="A12" s="201" t="s">
         <v>61</v>
       </c>
@@ -11639,10 +11641,10 @@
       <c r="V12" s="214"/>
       <c r="W12" s="215"/>
     </row>
-    <row r="13" spans="1:23" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" hidden="1" outlineLevel="1">
       <c r="A13" s="201"/>
     </row>
-    <row r="14" spans="1:23" ht="17" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="17" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A14" s="201" t="s">
         <v>62</v>
       </c>
@@ -11663,10 +11665,10 @@
       </c>
       <c r="V14" s="217"/>
     </row>
-    <row r="15" spans="1:23" ht="17" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" ht="17" hidden="1" outlineLevel="1" thickTop="1">
       <c r="D15" s="218"/>
     </row>
-    <row r="16" spans="1:23" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" hidden="1" outlineLevel="1">
       <c r="E16" s="219"/>
       <c r="H16" s="220"/>
       <c r="I16" s="219"/>
@@ -11675,12 +11677,12 @@
       <c r="N16" s="220"/>
       <c r="O16" s="219"/>
     </row>
-    <row r="17" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" hidden="1" outlineLevel="1">
       <c r="H17" s="221"/>
       <c r="K17" s="221"/>
       <c r="N17" s="221"/>
     </row>
-    <row r="18" spans="1:25" s="201" customFormat="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" s="201" customFormat="1" collapsed="1">
       <c r="C18" s="203">
         <v>2019</v>
       </c>
@@ -11745,7 +11747,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="19" spans="1:25" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" s="201" customFormat="1">
       <c r="C19" s="205" t="s">
         <v>56</v>
       </c>
@@ -11810,7 +11812,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:25" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" s="201" customFormat="1">
       <c r="A20" s="201" t="s">
         <v>61</v>
       </c>
@@ -11879,13 +11881,13 @@
       </c>
       <c r="Y20" s="222"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25">
       <c r="A21" s="201"/>
       <c r="D21" s="223"/>
       <c r="R21" s="223"/>
       <c r="Y21" s="223"/>
     </row>
-    <row r="22" spans="1:25" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" s="201" customFormat="1">
       <c r="A22" s="201" t="s">
         <v>66</v>
       </c>
@@ -11954,12 +11956,12 @@
       </c>
       <c r="Y22" s="222"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25">
       <c r="A23" s="201"/>
       <c r="R23" s="223"/>
       <c r="Y23" s="223"/>
     </row>
-    <row r="24" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="17" thickBot="1">
       <c r="A24" s="201" t="s">
         <v>67</v>
       </c>
@@ -12029,7 +12031,7 @@
       </c>
       <c r="Y24" s="223"/>
     </row>
-    <row r="25" spans="1:25" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="17" thickTop="1">
       <c r="D25" s="225"/>
       <c r="E25" s="225"/>
       <c r="F25" s="225"/>
@@ -12044,7 +12046,7 @@
       <c r="O25" s="225"/>
       <c r="R25" s="226"/>
     </row>
-    <row r="26" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="17" thickBot="1">
       <c r="D26" s="227"/>
       <c r="E26" s="227"/>
       <c r="F26" s="227"/>
@@ -12065,13 +12067,13 @@
       <c r="U26" s="227"/>
       <c r="V26" s="227"/>
     </row>
-    <row r="27" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="302" t="s">
+    <row r="27" spans="1:25" ht="17" thickBot="1">
+      <c r="D27" s="304" t="s">
         <v>99</v>
       </c>
-      <c r="E27" s="303"/>
-      <c r="F27" s="303"/>
-      <c r="G27" s="304"/>
+      <c r="E27" s="305"/>
+      <c r="F27" s="305"/>
+      <c r="G27" s="306"/>
       <c r="H27" s="228"/>
       <c r="I27" s="228"/>
       <c r="J27" s="228"/>
@@ -12088,13 +12090,13 @@
       <c r="U27" s="228"/>
       <c r="V27" s="228"/>
     </row>
-    <row r="28" spans="1:25" s="201" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" s="201" customFormat="1" ht="17" thickBot="1">
       <c r="A28" s="229" t="s">
         <v>68</v>
       </c>
       <c r="H28" s="230"/>
     </row>
-    <row r="29" spans="1:25" s="201" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" s="201" customFormat="1" ht="17" thickBot="1">
       <c r="A29" s="201" t="s">
         <v>69</v>
       </c>
@@ -12162,7 +12164,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="30" spans="1:25" s="201" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" s="201" customFormat="1" ht="17" thickBot="1">
       <c r="A30" s="201" t="s">
         <v>70</v>
       </c>
@@ -12230,7 +12232,7 @@
         <v>3.5486222936743741</v>
       </c>
     </row>
-    <row r="31" spans="1:25" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" s="201" customFormat="1">
       <c r="A31" s="201" t="s">
         <v>71</v>
       </c>
@@ -12298,7 +12300,7 @@
         <v>2.5704653170596177</v>
       </c>
     </row>
-    <row r="32" spans="1:25" s="201" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" s="201" customFormat="1" ht="17" thickBot="1">
       <c r="A32" s="201" t="s">
         <v>72</v>
       </c>
@@ -12366,13 +12368,13 @@
         <v>2.6447568091505178</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="E33" s="221"/>
       <c r="F33" s="221"/>
       <c r="G33" s="221"/>
       <c r="H33" s="221"/>
     </row>
-    <row r="34" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" s="201" customFormat="1">
       <c r="A34" s="229" t="s">
         <v>73</v>
       </c>
@@ -12381,7 +12383,7 @@
       <c r="G34" s="230"/>
       <c r="H34" s="230"/>
     </row>
-    <row r="35" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" s="201" customFormat="1">
       <c r="A35" s="201" t="s">
         <v>69</v>
       </c>
@@ -12449,7 +12451,7 @@
         <v>0.3725923633910791</v>
       </c>
     </row>
-    <row r="36" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" s="201" customFormat="1">
       <c r="A36" s="201" t="s">
         <v>70</v>
       </c>
@@ -12517,7 +12519,7 @@
         <v>0.59035130290895832</v>
       </c>
     </row>
-    <row r="37" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" s="201" customFormat="1">
       <c r="A37" s="201" t="s">
         <v>71</v>
       </c>
@@ -12585,7 +12587,7 @@
         <v>2.7785137221154201E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" s="201" customFormat="1">
       <c r="A38" s="201" t="s">
         <v>72</v>
       </c>
@@ -12653,7 +12655,7 @@
         <v>9.2711964788083634E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" s="201" customFormat="1">
       <c r="C39" s="235">
         <v>1</v>
       </c>
@@ -12718,10 +12720,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23">
       <c r="W40" s="215"/>
     </row>
-    <row r="41" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" s="201" customFormat="1">
       <c r="A41" s="201" t="s">
         <v>74</v>
       </c>
@@ -12789,7 +12791,7 @@
         <v>142047.62824417662</v>
       </c>
     </row>
-    <row r="42" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" s="201" customFormat="1">
       <c r="A42" s="201" t="s">
         <v>75</v>
       </c>
@@ -12857,7 +12859,7 @@
         <v>212980.1224004188</v>
       </c>
     </row>
-    <row r="43" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" s="201" customFormat="1">
       <c r="A43" s="201" t="s">
         <v>76</v>
       </c>
@@ -12925,7 +12927,7 @@
         <v>7260.9436098022998</v>
       </c>
     </row>
-    <row r="44" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" s="201" customFormat="1">
       <c r="A44" s="201" t="s">
         <v>77</v>
       </c>
@@ -12993,7 +12995,7 @@
         <v>2492.8164302816931</v>
       </c>
     </row>
-    <row r="45" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" s="201" customFormat="1">
       <c r="A45" s="201" t="s">
         <v>78</v>
       </c>
@@ -13061,7 +13063,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="46" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" s="201" customFormat="1">
       <c r="A46" s="201" t="s">
         <v>79</v>
       </c>
@@ -13129,7 +13131,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="47" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" s="201" customFormat="1">
       <c r="D47" s="222"/>
       <c r="E47" s="222"/>
       <c r="F47" s="222"/>
@@ -13143,7 +13145,7 @@
       <c r="N47" s="222"/>
       <c r="O47" s="222"/>
     </row>
-    <row r="48" spans="1:23" s="198" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" s="198" customFormat="1" ht="17" thickBot="1">
       <c r="A48" s="237" t="s">
         <v>80</v>
       </c>
@@ -13212,7 +13214,7 @@
         <v>366011.51068467938</v>
       </c>
     </row>
-    <row r="49" spans="1:23" s="241" customFormat="1" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" s="241" customFormat="1" ht="17" thickTop="1">
       <c r="A49" s="238" t="s">
         <v>81</v>
       </c>
@@ -13222,7 +13224,7 @@
       </c>
       <c r="D49" s="240"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23">
       <c r="C50" s="223"/>
       <c r="D50" s="223"/>
       <c r="E50" s="223"/>
@@ -13245,7 +13247,7 @@
       <c r="V50" s="223"/>
       <c r="W50" s="223"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23">
       <c r="A51" s="242" t="s">
         <v>82</v>
       </c>
@@ -13271,24 +13273,24 @@
       <c r="V51" s="215"/>
       <c r="W51" s="215"/>
     </row>
-    <row r="52" spans="1:23" s="201" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="300" t="s">
+    <row r="52" spans="1:23" s="201" customFormat="1">
+      <c r="A52" s="302" t="s">
         <v>83</v>
       </c>
-      <c r="B52" s="300"/>
-      <c r="C52" s="300"/>
-      <c r="D52" s="300"/>
+      <c r="B52" s="302"/>
+      <c r="C52" s="302"/>
+      <c r="D52" s="302"/>
       <c r="E52" s="236"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A53" s="301" t="s">
+    <row r="53" spans="1:23">
+      <c r="A53" s="303" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="301"/>
-      <c r="C53" s="301"/>
-      <c r="D53" s="301"/>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B53" s="303"/>
+      <c r="C53" s="303"/>
+      <c r="D53" s="303"/>
+    </row>
+    <row r="54" spans="1:23">
       <c r="A54" s="243" t="s">
         <v>85</v>
       </c>
@@ -13296,7 +13298,7 @@
       <c r="C54" s="245"/>
       <c r="D54" s="245"/>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23">
       <c r="D55" s="220"/>
     </row>
   </sheetData>
@@ -13322,7 +13324,7 @@
       <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="32.6640625" style="199" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" style="199" hidden="1" customWidth="1"/>
@@ -13336,42 +13338,42 @@
     <col min="25" max="16384" width="9.33203125" style="199"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="18">
       <c r="A1" s="265" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A2" s="198" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A3" s="198" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="200">
         <v>43697</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="201" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="299" t="s">
+    <row r="6" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1"/>
+    <row r="7" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="B7" s="301" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="299"/>
-      <c r="D7" s="299"/>
-      <c r="E7" s="299"/>
-      <c r="F7" s="299"/>
-    </row>
-    <row r="8" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="301"/>
+      <c r="D7" s="301"/>
+      <c r="E7" s="301"/>
+      <c r="F7" s="301"/>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="B8" s="203">
         <v>2019</v>
       </c>
@@ -13410,7 +13412,7 @@
       <c r="R8" s="246"/>
       <c r="S8" s="246"/>
     </row>
-    <row r="9" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="204"/>
       <c r="B9" s="205" t="s">
         <v>56</v>
@@ -13452,7 +13454,7 @@
       <c r="U9" s="207"/>
       <c r="V9" s="208"/>
     </row>
-    <row r="10" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A10" s="201" t="s">
         <v>59</v>
       </c>
@@ -13496,7 +13498,7 @@
       <c r="U10" s="207"/>
       <c r="V10" s="208"/>
     </row>
-    <row r="11" spans="1:22" ht="16.5" hidden="1" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="16.5" hidden="1" customHeight="1" outlineLevel="1" thickBot="1">
       <c r="A11" s="201" t="s">
         <v>50</v>
       </c>
@@ -13536,7 +13538,7 @@
       <c r="U11" s="207"/>
       <c r="V11" s="208"/>
     </row>
-    <row r="12" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A12" s="201" t="s">
         <v>61</v>
       </c>
@@ -13562,10 +13564,10 @@
       <c r="U12" s="214"/>
       <c r="V12" s="215"/>
     </row>
-    <row r="13" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A13" s="201"/>
     </row>
-    <row r="14" spans="1:22" ht="16.5" hidden="1" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="16.5" hidden="1" customHeight="1" outlineLevel="1" thickBot="1">
       <c r="A14" s="201" t="s">
         <v>62</v>
       </c>
@@ -13586,10 +13588,10 @@
       </c>
       <c r="U14" s="217"/>
     </row>
-    <row r="15" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="C15" s="218"/>
     </row>
-    <row r="16" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="D16" s="219"/>
       <c r="G16" s="220"/>
       <c r="H16" s="219"/>
@@ -13598,12 +13600,12 @@
       <c r="M16" s="220"/>
       <c r="N16" s="219"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="G17" s="221"/>
       <c r="J17" s="221"/>
       <c r="M17" s="221"/>
     </row>
-    <row r="18" spans="1:24" s="201" customFormat="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" s="201" customFormat="1" collapsed="1">
       <c r="B18" s="203">
         <v>2019</v>
       </c>
@@ -13668,7 +13670,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="19" spans="1:24" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" s="201" customFormat="1">
       <c r="B19" s="205" t="s">
         <v>56</v>
       </c>
@@ -13733,7 +13735,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:24" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" s="201" customFormat="1">
       <c r="A20" s="201" t="s">
         <v>61</v>
       </c>
@@ -13802,13 +13804,13 @@
       </c>
       <c r="X20" s="222"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24">
       <c r="A21" s="201"/>
       <c r="C21" s="223"/>
       <c r="Q21" s="223"/>
       <c r="X21" s="223"/>
     </row>
-    <row r="22" spans="1:24" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" s="201" customFormat="1">
       <c r="A22" s="201" t="s">
         <v>66</v>
       </c>
@@ -13877,12 +13879,12 @@
       </c>
       <c r="X22" s="222"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24">
       <c r="A23" s="201"/>
       <c r="Q23" s="223"/>
       <c r="X23" s="223"/>
     </row>
-    <row r="24" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="17" thickBot="1">
       <c r="A24" s="201" t="s">
         <v>67</v>
       </c>
@@ -13951,7 +13953,7 @@
       </c>
       <c r="X24" s="223"/>
     </row>
-    <row r="25" spans="1:24" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" ht="17" thickTop="1">
       <c r="C25" s="225"/>
       <c r="D25" s="225"/>
       <c r="E25" s="225"/>
@@ -13966,7 +13968,7 @@
       <c r="N25" s="225"/>
       <c r="Q25" s="226"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24">
       <c r="C26" s="227"/>
       <c r="D26" s="227"/>
       <c r="E26" s="227"/>
@@ -13987,7 +13989,7 @@
       <c r="T26" s="227"/>
       <c r="U26" s="227"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24">
       <c r="C27" s="228"/>
       <c r="D27" s="228"/>
       <c r="E27" s="228"/>
@@ -14008,7 +14010,7 @@
       <c r="T27" s="228"/>
       <c r="U27" s="228"/>
     </row>
-    <row r="28" spans="1:24" s="201" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" s="201" customFormat="1" ht="17" thickBot="1">
       <c r="A28" s="229" t="s">
         <v>68</v>
       </c>
@@ -14018,7 +14020,7 @@
       <c r="F28" s="230"/>
       <c r="G28" s="230"/>
     </row>
-    <row r="29" spans="1:24" s="201" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" s="201" customFormat="1" ht="17" thickBot="1">
       <c r="A29" s="201" t="s">
         <v>69</v>
       </c>
@@ -14087,7 +14089,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="30" spans="1:24" s="201" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" s="201" customFormat="1" ht="17" thickBot="1">
       <c r="A30" s="201" t="s">
         <v>70</v>
       </c>
@@ -14173,7 +14175,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="31" spans="1:24" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" s="201" customFormat="1">
       <c r="A31" s="201" t="s">
         <v>71</v>
       </c>
@@ -14260,7 +14262,7 @@
         <v>3.739431234198201</v>
       </c>
     </row>
-    <row r="32" spans="1:24" s="201" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" s="201" customFormat="1" ht="17" thickBot="1">
       <c r="A32" s="201" t="s">
         <v>72</v>
       </c>
@@ -14347,13 +14349,13 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22">
       <c r="D33" s="221"/>
       <c r="E33" s="221"/>
       <c r="F33" s="221"/>
       <c r="G33" s="221"/>
     </row>
-    <row r="34" spans="1:22" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" s="201" customFormat="1">
       <c r="A34" s="229" t="s">
         <v>73</v>
       </c>
@@ -14362,7 +14364,7 @@
       <c r="F34" s="230"/>
       <c r="G34" s="230"/>
     </row>
-    <row r="35" spans="1:22" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" s="201" customFormat="1">
       <c r="A35" s="201" t="s">
         <v>69</v>
       </c>
@@ -14430,7 +14432,7 @@
         <v>0.3725923633910791</v>
       </c>
     </row>
-    <row r="36" spans="1:22" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" s="201" customFormat="1">
       <c r="A36" s="201" t="s">
         <v>70</v>
       </c>
@@ -14498,7 +14500,7 @@
         <v>0.59035130290895832</v>
       </c>
     </row>
-    <row r="37" spans="1:22" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" s="201" customFormat="1">
       <c r="A37" s="201" t="s">
         <v>71</v>
       </c>
@@ -14566,7 +14568,7 @@
         <v>2.7785137221154201E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:22" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" s="201" customFormat="1">
       <c r="A38" s="201" t="s">
         <v>72</v>
       </c>
@@ -14634,7 +14636,7 @@
         <v>9.2711964788083634E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:22" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" s="201" customFormat="1">
       <c r="B39" s="235">
         <v>1</v>
       </c>
@@ -14699,10 +14701,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22">
       <c r="V40" s="215"/>
     </row>
-    <row r="41" spans="1:22" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" s="201" customFormat="1">
       <c r="A41" s="201" t="s">
         <v>74</v>
       </c>
@@ -14791,7 +14793,7 @@
         <v>142047.62824417662</v>
       </c>
     </row>
-    <row r="42" spans="1:22" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" s="201" customFormat="1">
       <c r="A42" s="201" t="s">
         <v>75</v>
       </c>
@@ -14880,7 +14882,7 @@
         <v>204060.15524735671</v>
       </c>
     </row>
-    <row r="43" spans="1:22" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" s="201" customFormat="1">
       <c r="A43" s="201" t="s">
         <v>76</v>
       </c>
@@ -14969,7 +14971,7 @@
         <v>10562.989955182818</v>
       </c>
     </row>
-    <row r="44" spans="1:22" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" s="201" customFormat="1">
       <c r="A44" s="201" t="s">
         <v>77</v>
       </c>
@@ -15058,7 +15060,7 @@
         <v>3534.5637758501125</v>
       </c>
     </row>
-    <row r="45" spans="1:22" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" s="201" customFormat="1">
       <c r="A45" s="201" t="s">
         <v>78</v>
       </c>
@@ -15126,7 +15128,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="46" spans="1:22" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" s="201" customFormat="1">
       <c r="A46" s="201" t="s">
         <v>79</v>
       </c>
@@ -15194,7 +15196,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="47" spans="1:22" s="201" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" s="201" customFormat="1">
       <c r="C47" s="222"/>
       <c r="D47" s="222"/>
       <c r="E47" s="222"/>
@@ -15208,7 +15210,7 @@
       <c r="M47" s="222"/>
       <c r="N47" s="222"/>
     </row>
-    <row r="48" spans="1:22" s="198" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" s="198" customFormat="1" ht="17" thickBot="1">
       <c r="A48" s="237" t="s">
         <v>80</v>
       </c>
@@ -15297,7 +15299,7 @@
         <v>361435.3372225663</v>
       </c>
     </row>
-    <row r="49" spans="3:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:3" ht="17" thickTop="1">
       <c r="C49" s="220"/>
     </row>
   </sheetData>
@@ -15313,11 +15315,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07D768D-8F1F-4F37-877B-25A0898D4A0D}">
   <dimension ref="C1:AX46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="N44" sqref="N44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="2.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" style="1" customWidth="1"/>
@@ -15371,13 +15373,13 @@
     <col min="51" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:50" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="305" t="s">
+    <row r="1" spans="3:50" ht="16" thickBot="1">
+      <c r="E1" s="307" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="305"/>
-      <c r="G1" s="305"/>
-      <c r="H1" s="305"/>
+      <c r="F1" s="307"/>
+      <c r="G1" s="307"/>
+      <c r="H1" s="307"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -15387,43 +15389,43 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="3:50" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="306" t="s">
+    <row r="2" spans="3:50" ht="15" customHeight="1">
+      <c r="C2" s="308" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="309" t="s">
+      <c r="D2" s="311" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="312" t="s">
+      <c r="E2" s="314" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="313"/>
-      <c r="G2" s="313"/>
-      <c r="H2" s="314"/>
-      <c r="I2" s="315" t="s">
+      <c r="F2" s="315"/>
+      <c r="G2" s="315"/>
+      <c r="H2" s="316"/>
+      <c r="I2" s="317" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="316"/>
-      <c r="K2" s="316"/>
-      <c r="L2" s="316"/>
-      <c r="M2" s="316"/>
-      <c r="N2" s="316"/>
-      <c r="O2" s="316"/>
-      <c r="P2" s="316"/>
-      <c r="Q2" s="316"/>
-      <c r="R2" s="316"/>
-      <c r="S2" s="316"/>
-      <c r="T2" s="317"/>
+      <c r="J2" s="318"/>
+      <c r="K2" s="318"/>
+      <c r="L2" s="318"/>
+      <c r="M2" s="318"/>
+      <c r="N2" s="318"/>
+      <c r="O2" s="318"/>
+      <c r="P2" s="318"/>
+      <c r="Q2" s="318"/>
+      <c r="R2" s="318"/>
+      <c r="S2" s="318"/>
+      <c r="T2" s="319"/>
       <c r="U2" s="4"/>
       <c r="V2" s="5"/>
-      <c r="W2" s="326" t="s">
+      <c r="W2" s="328" t="s">
         <v>4</v>
       </c>
-      <c r="X2" s="327"/>
-      <c r="Y2" s="327"/>
-      <c r="Z2" s="327"/>
-      <c r="AA2" s="327"/>
-      <c r="AB2" s="328"/>
+      <c r="X2" s="329"/>
+      <c r="Y2" s="329"/>
+      <c r="Z2" s="329"/>
+      <c r="AA2" s="329"/>
+      <c r="AB2" s="330"/>
       <c r="AC2" s="6"/>
       <c r="AD2" s="6"/>
       <c r="AE2" s="6"/>
@@ -15433,49 +15435,49 @@
       <c r="AI2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AJ2" s="318" t="s">
+      <c r="AJ2" s="320" t="s">
         <v>6</v>
       </c>
-      <c r="AK2" s="317"/>
-      <c r="AM2" s="319" t="s">
+      <c r="AK2" s="319"/>
+      <c r="AM2" s="321" t="s">
         <v>7</v>
       </c>
-      <c r="AN2" s="320"/>
-      <c r="AP2" s="321" t="s">
+      <c r="AN2" s="322"/>
+      <c r="AP2" s="323" t="s">
         <v>8</v>
       </c>
-      <c r="AQ2" s="322"/>
+      <c r="AQ2" s="324"/>
       <c r="AR2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AS2" s="318" t="s">
+      <c r="AS2" s="320" t="s">
         <v>9</v>
       </c>
-      <c r="AT2" s="317"/>
-    </row>
-    <row r="3" spans="3:50" x14ac:dyDescent="0.2">
-      <c r="C3" s="307"/>
-      <c r="D3" s="310"/>
+      <c r="AT2" s="319"/>
+    </row>
+    <row r="3" spans="3:50">
+      <c r="C3" s="309"/>
+      <c r="D3" s="312"/>
       <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="323" t="s">
+      <c r="I3" s="325" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="324"/>
-      <c r="K3" s="324"/>
-      <c r="L3" s="324"/>
-      <c r="M3" s="324"/>
-      <c r="N3" s="324"/>
-      <c r="O3" s="324"/>
-      <c r="P3" s="324"/>
-      <c r="Q3" s="324"/>
-      <c r="R3" s="324"/>
-      <c r="S3" s="324"/>
-      <c r="T3" s="325"/>
+      <c r="J3" s="326"/>
+      <c r="K3" s="326"/>
+      <c r="L3" s="326"/>
+      <c r="M3" s="326"/>
+      <c r="N3" s="326"/>
+      <c r="O3" s="326"/>
+      <c r="P3" s="326"/>
+      <c r="Q3" s="326"/>
+      <c r="R3" s="326"/>
+      <c r="S3" s="326"/>
+      <c r="T3" s="327"/>
       <c r="U3" s="11"/>
       <c r="V3" s="12"/>
       <c r="W3" s="13"/>
@@ -15503,9 +15505,9 @@
       <c r="AS3" s="22"/>
       <c r="AT3" s="23"/>
     </row>
-    <row r="4" spans="3:50" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="307"/>
-      <c r="D4" s="310"/>
+    <row r="4" spans="3:50" ht="16" thickBot="1">
+      <c r="C4" s="309"/>
+      <c r="D4" s="312"/>
       <c r="E4" s="24"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
@@ -15553,9 +15555,9 @@
       <c r="AS4" s="42"/>
       <c r="AT4" s="43"/>
     </row>
-    <row r="5" spans="3:50" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="308"/>
-      <c r="D5" s="311"/>
+    <row r="5" spans="3:50" ht="16" thickBot="1">
+      <c r="C5" s="310"/>
+      <c r="D5" s="313"/>
       <c r="E5" s="44" t="s">
         <v>16</v>
       </c>
@@ -15632,7 +15634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:50" ht="17" thickBot="1">
       <c r="C6" s="62">
         <v>2002</v>
       </c>
@@ -15689,7 +15691,7 @@
         <v>51920735</v>
       </c>
     </row>
-    <row r="7" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:50" ht="17" thickBot="1">
       <c r="C7" s="77">
         <v>2003</v>
       </c>
@@ -15746,7 +15748,7 @@
         <v>47913881</v>
       </c>
     </row>
-    <row r="8" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:50" ht="17" thickBot="1">
       <c r="C8" s="77">
         <v>2004</v>
       </c>
@@ -15803,7 +15805,7 @@
         <v>57699388</v>
       </c>
     </row>
-    <row r="9" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:50" ht="17" thickBot="1">
       <c r="C9" s="77">
         <v>2005</v>
       </c>
@@ -15860,7 +15862,7 @@
         <v>60711890</v>
       </c>
     </row>
-    <row r="10" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:50" ht="17" thickBot="1">
       <c r="C10" s="77">
         <v>2006</v>
       </c>
@@ -15917,7 +15919,7 @@
         <v>66830318</v>
       </c>
     </row>
-    <row r="11" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:50" ht="17" thickBot="1">
       <c r="C11" s="77">
         <v>2007</v>
       </c>
@@ -15974,7 +15976,7 @@
         <v>71554741</v>
       </c>
     </row>
-    <row r="12" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:50" ht="17" thickBot="1">
       <c r="C12" s="77">
         <v>2008</v>
       </c>
@@ -16032,7 +16034,7 @@
         <v>74933113</v>
       </c>
     </row>
-    <row r="13" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:50" ht="17" thickBot="1">
       <c r="C13" s="77">
         <v>2009</v>
       </c>
@@ -16090,7 +16092,7 @@
         <v>72279443</v>
       </c>
     </row>
-    <row r="14" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:50" ht="17" thickBot="1">
       <c r="C14" s="77">
         <v>2010</v>
       </c>
@@ -16148,7 +16150,7 @@
         <v>73797524</v>
       </c>
     </row>
-    <row r="15" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:50" ht="17" thickBot="1">
       <c r="C15" s="77">
         <v>2011</v>
       </c>
@@ -16205,7 +16207,7 @@
         <v>76318219</v>
       </c>
     </row>
-    <row r="16" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:50" ht="17" thickBot="1">
       <c r="C16" s="77">
         <v>2012</v>
       </c>
@@ -16262,7 +16264,7 @@
         <v>72477565</v>
       </c>
     </row>
-    <row r="17" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:50" ht="17" thickBot="1">
       <c r="C17" s="77">
         <v>2013</v>
       </c>
@@ -16319,7 +16321,7 @@
         <v>72751921</v>
       </c>
     </row>
-    <row r="18" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:50" ht="17" thickBot="1">
       <c r="C18" s="77">
         <v>2014</v>
       </c>
@@ -16377,7 +16379,7 @@
         <v>73609147</v>
       </c>
     </row>
-    <row r="19" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:50" ht="17" thickBot="1">
       <c r="C19" s="77">
         <v>2015</v>
       </c>
@@ -16437,7 +16439,7 @@
         <v>76463422</v>
       </c>
     </row>
-    <row r="20" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:50" ht="17" thickBot="1">
       <c r="C20" s="77">
         <v>2016</v>
       </c>
@@ -16494,7 +16496,7 @@
         <v>78517133</v>
       </c>
     </row>
-    <row r="21" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:50" ht="17" thickBot="1">
       <c r="C21" s="77">
         <v>2017</v>
       </c>
@@ -16551,7 +16553,7 @@
         <v>81601062</v>
       </c>
     </row>
-    <row r="22" spans="3:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:50" ht="17" thickBot="1">
       <c r="C22" s="77">
         <v>2018</v>
       </c>
@@ -16642,7 +16644,7 @@
         <v>81569178</v>
       </c>
     </row>
-    <row r="23" spans="3:50" s="124" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:50" s="124" customFormat="1">
       <c r="C23" s="100">
         <v>2019</v>
       </c>
@@ -16766,7 +16768,7 @@
         <v>3.444588309184593E-3</v>
       </c>
     </row>
-    <row r="24" spans="3:50" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:50">
       <c r="C24" s="77">
         <v>2020</v>
       </c>
@@ -16894,7 +16896,7 @@
         <v>2.7793759426366572E-2</v>
       </c>
     </row>
-    <row r="25" spans="3:50" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:50">
       <c r="C25" s="77">
         <v>2021</v>
       </c>
@@ -17018,7 +17020,7 @@
         <v>3.1417339513762049E-2</v>
       </c>
     </row>
-    <row r="26" spans="3:50" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:50">
       <c r="C26" s="77">
         <v>2022</v>
       </c>
@@ -17142,7 +17144,7 @@
         <v>9.1960450733762026E-3</v>
       </c>
     </row>
-    <row r="27" spans="3:50" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:50">
       <c r="C27" s="77">
         <v>2023</v>
       </c>
@@ -17266,7 +17268,7 @@
         <v>5.4151845652609682E-3</v>
       </c>
     </row>
-    <row r="28" spans="3:50" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:50">
       <c r="C28" s="77">
         <v>2024</v>
       </c>
@@ -17390,7 +17392,7 @@
         <v>1.3181173790305444E-2</v>
       </c>
     </row>
-    <row r="29" spans="3:50" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:50">
       <c r="C29" s="77">
         <v>2025</v>
       </c>
@@ -17514,7 +17516,7 @@
         <v>5.4861130765003199E-3</v>
       </c>
     </row>
-    <row r="30" spans="3:50" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:50">
       <c r="C30" s="77">
         <v>2026</v>
       </c>
@@ -17638,7 +17640,7 @@
         <v>9.4176304900555272E-3</v>
       </c>
     </row>
-    <row r="31" spans="3:50" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:50">
       <c r="C31" s="77">
         <v>2027</v>
       </c>
@@ -17762,7 +17764,7 @@
         <v>8.0272146710083717E-3</v>
       </c>
     </row>
-    <row r="32" spans="3:50" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:50">
       <c r="C32" s="77">
         <v>2028</v>
       </c>
@@ -17886,7 +17888,7 @@
         <v>1.299990258212577E-2</v>
       </c>
     </row>
-    <row r="33" spans="3:46" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:46">
       <c r="C33" s="77">
         <v>2029</v>
       </c>
@@ -18010,7 +18012,7 @@
         <v>9.1473171593530554E-3</v>
       </c>
     </row>
-    <row r="34" spans="3:46" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:46">
       <c r="C34" s="77">
         <v>2030</v>
       </c>
@@ -18134,7 +18136,7 @@
         <v>1.0233603798094053E-2</v>
       </c>
     </row>
-    <row r="35" spans="3:46" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:46">
       <c r="C35" s="77">
         <v>2031</v>
       </c>
@@ -18258,7 +18260,7 @@
         <v>9.5987724365873012E-3</v>
       </c>
     </row>
-    <row r="36" spans="3:46" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:46">
       <c r="C36" s="77">
         <v>2032</v>
       </c>
@@ -18382,7 +18384,7 @@
         <v>1.1260127577234977E-2</v>
       </c>
     </row>
-    <row r="37" spans="3:46" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:46">
       <c r="C37" s="77">
         <v>2033</v>
       </c>
@@ -18506,7 +18508,7 @@
         <v>8.1999860882431396E-3</v>
       </c>
     </row>
-    <row r="38" spans="3:46" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:46">
       <c r="C38" s="77">
         <v>2034</v>
       </c>
@@ -18630,7 +18632,7 @@
         <v>6.7986463485594393E-3</v>
       </c>
     </row>
-    <row r="39" spans="3:46" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:46">
       <c r="C39" s="77">
         <v>2035</v>
       </c>
@@ -18754,7 +18756,7 @@
         <v>1.0830198537625747E-2</v>
       </c>
     </row>
-    <row r="40" spans="3:46" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:46">
       <c r="C40" s="77">
         <v>2036</v>
       </c>
@@ -18878,7 +18880,7 @@
         <v>1.1441322637268105E-2</v>
       </c>
     </row>
-    <row r="41" spans="3:46" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:46" ht="16" thickBot="1">
       <c r="C41" s="129">
         <v>2037</v>
       </c>
@@ -19002,7 +19004,8 @@
         <v>9.8391193882683518E-3</v>
       </c>
     </row>
-    <row r="43" spans="3:46" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:46">
+      <c r="J43" s="299"/>
       <c r="Q43" s="151">
         <v>9.9274108603917277E-3</v>
       </c>
@@ -19036,7 +19039,17 @@
         <v>9.5371797017385074E-3</v>
       </c>
     </row>
-    <row r="46" spans="3:46" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:46">
+      <c r="D44" s="300">
+        <f>(I23/D13)^(1/COUNT(D14:D23))-1</f>
+        <v>1.7383537429585427E-2</v>
+      </c>
+      <c r="J44" s="300">
+        <f>(I41/I22)^(1/COUNT(I23:I41))-1</f>
+        <v>1.1137054428210336E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="3:46">
       <c r="AC46" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>